<commit_message>
Correcting non binary column
</commit_message>
<xml_diff>
--- a/example-vector.xlsx
+++ b/example-vector.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planeacionnacional-my.sharepoint.com/personal/cmayorquin_dnp_gov_co/Documents/DIDE/2019/Data Science Projects/Innovation-Index-Algorithms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScmayorquinS\OneDrive - Departamento Nacional de Planeacion\DIDE\2019\Data Science Projects\Innovation-Index-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D3164B7-5A40-4F98-B4EE-BB460631E24A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8D3164B7-5A40-4F98-B4EE-BB460631E24A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{CB6A59F3-2505-4487-9BB7-22DCA08B0337}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{DF588736-EEBA-4653-A60D-0A64F03C21D6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>1A</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>60A;60B;60C;60D;61A1;61A2;61A3;61B1</t>
+  </si>
+  <si>
+    <t>1A;1B;1C;1D;1E;1G;2A;2B;2C;2D</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1052,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1062,7 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changing example for common case
</commit_message>
<xml_diff>
--- a/example-vector.xlsx
+++ b/example-vector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScmayorquinS\OneDrive - Departamento Nacional de Planeacion\DIDE\2019\Data Science Projects\Innovation-Index-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{8D3164B7-5A40-4F98-B4EE-BB460631E24A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{CB6A59F3-2505-4487-9BB7-22DCA08B0337}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{8D3164B7-5A40-4F98-B4EE-BB460631E24A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0567F9C8-7C9F-4533-BA14-14FF17D5ED07}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{DF588736-EEBA-4653-A60D-0A64F03C21D6}"/>
   </bookViews>
@@ -127,10 +127,10 @@
     <t>var 2</t>
   </si>
   <si>
-    <t>60A;60B;60C;60D;61A1;61A2;61A3;61B1</t>
-  </si>
-  <si>
     <t>1A;1B;1C;1D;1E;1G;2A;2B;2C;2D</t>
+  </si>
+  <si>
+    <t>4A;4B;4C;4D</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1062,7 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>